<commit_message>
Window notification created and added
</commit_message>
<xml_diff>
--- a/planilha/LME_media_mensal.xlsx
+++ b/planilha/LME_media_mensal.xlsx
@@ -1,37 +1,90 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+  <si>
+    <t>Mês</t>
+  </si>
+  <si>
+    <t>Cobre</t>
+  </si>
+  <si>
+    <t>Zinco</t>
+  </si>
+  <si>
+    <t>Aluminio</t>
+  </si>
+  <si>
+    <t>Chumbo</t>
+  </si>
+  <si>
+    <t>Estanho</t>
+  </si>
+  <si>
+    <t>Niquel</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Fev</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Abr</t>
+  </si>
+  <si>
+    <t>Mai</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Ago</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +99,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,307 +415,290 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Mês</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Cobre</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Zinco</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Aluminio</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Chumbo</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Estanho</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Niquel</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Jan</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
         <v>54.114</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>19.983</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>16.617</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>12.969</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>231.324</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>123.503</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Fev</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
         <v>51.621</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>18.925</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>16.926</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>11.939</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>229.066</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>125.504</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Mar</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
         <v>50.983</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>19.782</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>17.617</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>11.751</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>220.527</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>188.53</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Abr</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
         <v>48.327</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>20.713</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>15.457</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>11.376</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>204.864</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>157.972</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Mai</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
         <v>46.455</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>18.646</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>14.02</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>10.644</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>178.482</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>138.709</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Jun</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
         <v>47.171</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>19.024</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>13.379</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>10.794</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>165.937</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>134.923</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Jul</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
         <v>47.171</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>19.024</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>13.379</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>10.794</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>165.937</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>134.923</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Ago</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
         <v>41.803</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>16.434</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>12.57</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>10.094</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>141.503</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>115.758</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Ago</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
         <v>41.803</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>16.434</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>12.57</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>10.094</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>141.503</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>115.758</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Ago</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
         <v>41.803</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>16.434</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>12.57</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>10.094</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>141.503</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>115.758</v>
       </c>
     </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>40.946</v>
+      </c>
+      <c r="C12">
+        <v>17.76</v>
+      </c>
+      <c r="D12">
+        <v>12.742</v>
+      </c>
+      <c r="E12">
+        <v>10.653</v>
+      </c>
+      <c r="F12">
+        <v>130.281</v>
+      </c>
+      <c r="G12">
+        <v>119.847</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>